<commit_message>
Alle restlichen communication_links hinzugefügt
</commit_message>
<xml_diff>
--- a/Threagile_fullrun/tags.xlsx
+++ b/Threagile_fullrun/tags.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Element</t>
   </si>
@@ -52,9 +52,15 @@
     <t>DC1</t>
   </si>
   <si>
+    <t>DC1-to-NTP</t>
+  </si>
+  <si>
     <t>DC2</t>
   </si>
   <si>
+    <t>DC2-to-DC1</t>
+  </si>
+  <si>
     <t>ES1</t>
   </si>
   <si>
@@ -103,6 +109,9 @@
     <t>FW4-to-FW3</t>
   </si>
   <si>
+    <t>NTP</t>
+  </si>
+  <si>
     <t>OS1</t>
   </si>
   <si>
@@ -130,6 +139,9 @@
     <t>R2-to-ES1</t>
   </si>
   <si>
+    <t>R2-to-DC2-NTP</t>
+  </si>
+  <si>
     <t>R3</t>
   </si>
   <si>
@@ -163,15 +175,24 @@
     <t>S1-to-R3</t>
   </si>
   <si>
+    <t>S1-to-R2-NTP</t>
+  </si>
+  <si>
     <t>S2</t>
   </si>
   <si>
+    <t>S2-to-DC1</t>
+  </si>
+  <si>
     <t>S3</t>
   </si>
   <si>
     <t>S3-to-FW4</t>
   </si>
   <si>
+    <t>S3-to-DC1</t>
+  </si>
+  <si>
     <t>S4</t>
   </si>
   <si>
@@ -190,13 +211,22 @@
     <t>S4-to-FW4</t>
   </si>
   <si>
+    <t>S4-to-DC1-NTP</t>
+  </si>
+  <si>
     <t>S4-to-DC1</t>
   </si>
   <si>
     <t>S5</t>
   </si>
   <si>
+    <t>S5-to-DC1</t>
+  </si>
+  <si>
     <t>S6</t>
+  </si>
+  <si>
+    <t>S6-to-DC1</t>
   </si>
   <si>
     <t>TI1</t>
@@ -679,9 +709,7 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
@@ -713,11 +741,11 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
@@ -781,7 +809,9 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
@@ -809,13 +839,9 @@
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
@@ -833,9 +859,13 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
@@ -863,9 +893,7 @@
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
@@ -884,12 +912,12 @@
         <v>31</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
@@ -897,7 +925,9 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
@@ -907,9 +937,7 @@
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
@@ -918,7 +946,9 @@
         <v>34</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -939,7 +969,9 @@
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
@@ -959,9 +991,7 @@
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
@@ -991,9 +1021,7 @@
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
@@ -1003,7 +1031,9 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
@@ -1021,9 +1051,7 @@
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1035,7 +1063,9 @@
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
@@ -1063,7 +1093,9 @@
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -1074,9 +1106,7 @@
         <v>49</v>
       </c>
       <c r="B44" s="1"/>
-      <c r="C44" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -1087,9 +1117,7 @@
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
@@ -1111,9 +1139,7 @@
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F47" s="1"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
@@ -1130,7 +1156,9 @@
         <v>54</v>
       </c>
       <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
+      <c r="C49" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -1151,7 +1179,9 @@
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
+      <c r="D51" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
     </row>
@@ -1180,21 +1210,19 @@
         <v>59</v>
       </c>
       <c r="B54" s="1"/>
-      <c r="C54" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
+      <c r="F54" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B55" s="1"/>
-      <c r="C55" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -1205,9 +1233,7 @@
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
@@ -1217,9 +1243,7 @@
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
     </row>
@@ -1228,9 +1252,7 @@
         <v>63</v>
       </c>
       <c r="B58" s="1"/>
-      <c r="C58" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -1250,9 +1272,7 @@
         <v>65</v>
       </c>
       <c r="B60" s="1"/>
-      <c r="C60" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -1308,24 +1328,20 @@
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
-      <c r="E65" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="E65" s="1"/>
       <c r="F65" s="1"/>
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B66" s="1"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+      <c r="D66" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E66" s="1"/>
-      <c r="F66" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F66" s="1"/>
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
@@ -1344,10 +1360,10 @@
         <v>73</v>
       </c>
       <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C68" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
@@ -1356,14 +1372,10 @@
         <v>74</v>
       </c>
       <c r="B69" s="1"/>
-      <c r="C69" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
-      <c r="F69" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F69" s="1"/>
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
@@ -1376,6 +1388,126 @@
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" s="1"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
     </row>
   </sheetData>
   <pageSetup orientation="landscape" paperSize="9"/>

</xml_diff>